<commit_message>
updatedcode bulk customer delete
</commit_message>
<xml_diff>
--- a/src/views/apps/freshlist/UploadFormats/CreateCustomerSample.xlsx
+++ b/src/views/apps/freshlist/UploadFormats/CreateCustomerSample.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="103">
   <si>
     <t>CompanyName</t>
   </si>
@@ -317,13 +317,19 @@
   </si>
   <si>
     <t>password</t>
+  </si>
+  <si>
+    <t>gstNumber</t>
+  </si>
+  <si>
+    <t>17CMRPS9572E1Z7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -331,13 +337,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -352,10 +376,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -688,762 +718,779 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AI7"/>
+  <dimension ref="A1:AJ7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="22.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="20.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="36.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="22.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="7.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="22.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="24.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="8.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="16384" width="9" style="1"/>
+    <col min="2" max="2" width="22.375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="36.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="22.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="22.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="24.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="8.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:36">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:35">
+    <row r="2" spans="1:36">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>15</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>1000000</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>15</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I2" s="1">
+      <c r="J2" s="1">
         <v>6232390353</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M2" s="1">
+      <c r="N2" s="1">
         <v>1789654123012</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="P2" s="1">
+      <c r="Q2" s="1">
         <v>452015</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="X2" s="1">
+      <c r="Y2" s="1">
         <v>123456</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="Z2" s="1">
+      <c r="AA2" s="1">
         <v>450129</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AE2" s="1" t="s">
+      <c r="AF2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AG2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AG2" s="1" t="s">
+      <c r="AH2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AH2" s="1" t="s">
+      <c r="AI2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AI2" s="1" t="s">
+      <c r="AJ2" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:35">
+    <row r="3" spans="1:36">
       <c r="A3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="1">
+      <c r="J3" s="1">
         <v>7854126980</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="M3" s="1">
+      <c r="N3" s="1">
         <v>1789654123012</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="P3" s="1">
+      <c r="Q3" s="1">
         <v>452015</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="W3" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="W3" s="1" t="s">
+      <c r="X3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="X3" s="1">
+      <c r="Y3" s="1">
         <v>123456</v>
       </c>
-      <c r="Y3" s="1" t="s">
+      <c r="Z3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="Z3" s="1">
+      <c r="AA3" s="1">
         <v>450128</v>
       </c>
-      <c r="AA3" s="1" t="s">
+      <c r="AB3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AB3" s="1" t="s">
+      <c r="AC3" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="AD3" s="1" t="s">
+      <c r="AE3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AE3" s="1" t="s">
+      <c r="AF3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AF3" s="1" t="s">
+      <c r="AG3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AG3" s="1" t="s">
+      <c r="AH3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AH3" s="1" t="s">
+      <c r="AI3" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AI3" s="1" t="s">
+      <c r="AJ3" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:36">
       <c r="A4" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I4" s="1">
+      <c r="J4" s="1">
         <v>7854126980</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="M4" s="1">
+      <c r="N4" s="1">
         <v>1789654123012</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="P4" s="1">
+      <c r="Q4" s="1">
         <v>452015</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="S4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="T4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="T4" s="1" t="s">
+      <c r="U4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="V4" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="W4" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="W4" s="1" t="s">
+      <c r="X4" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="X4" s="1">
+      <c r="Y4" s="1">
         <v>123456</v>
       </c>
-      <c r="Y4" s="1" t="s">
+      <c r="Z4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="Z4" s="1">
+      <c r="AA4" s="1">
         <v>450127</v>
       </c>
-      <c r="AA4" s="1" t="s">
+      <c r="AB4" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AB4" s="1" t="s">
+      <c r="AC4" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AD4" s="1" t="s">
+      <c r="AE4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AE4" s="1" t="s">
+      <c r="AF4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AF4" s="1" t="s">
+      <c r="AG4" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AG4" s="1" t="s">
+      <c r="AH4" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AH4" s="1" t="s">
+      <c r="AI4" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AI4" s="1" t="s">
+      <c r="AJ4" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:35">
+    <row r="5" spans="1:36">
       <c r="A5" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>30</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5" s="1">
         <v>1000000</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="1">
         <v>30</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="I5" s="1">
+      <c r="J5" s="1">
         <v>9131662204</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="M5" s="1">
+      <c r="N5" s="1">
         <v>111122223333</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="O5" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="P5" s="1">
+      <c r="Q5" s="1">
         <v>452001</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="R5" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="R5" s="1" t="s">
+      <c r="S5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="S5" s="1" t="s">
+      <c r="T5" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="T5" s="1" t="s">
+      <c r="U5" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="U5" s="1" t="s">
+      <c r="V5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="V5" s="1" t="s">
+      <c r="W5" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="W5" s="1" t="s">
+      <c r="X5" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="X5" s="1">
+      <c r="Y5" s="1">
         <v>123456</v>
       </c>
-      <c r="Y5" s="1" t="s">
+      <c r="Z5" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="Z5" s="1">
+      <c r="AA5" s="1">
         <v>200000</v>
       </c>
-      <c r="AA5" s="1" t="s">
+      <c r="AB5" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AB5" s="1" t="s">
+      <c r="AC5" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AC5" s="1" t="s">
+      <c r="AD5" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="AD5" s="1" t="s">
+      <c r="AE5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AE5" s="1" t="s">
+      <c r="AF5" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="AF5" s="1" t="s">
+      <c r="AG5" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="AG5" s="1" t="s">
+      <c r="AH5" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AH5" s="1" t="s">
+      <c r="AI5" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AI5" s="1" t="s">
+      <c r="AJ5" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:35">
+    <row r="6" spans="1:36">
       <c r="A6" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I6" s="1">
+      <c r="J6" s="1">
         <v>7854126980</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="M6" s="1">
+      <c r="N6" s="1">
         <v>1789654123014</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="O6" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="P6" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="P6" s="1">
+      <c r="Q6" s="1">
         <v>452016</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="R6" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="R6" s="1" t="s">
+      <c r="S6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="S6" s="1" t="s">
+      <c r="T6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="T6" s="1" t="s">
+      <c r="U6" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="U6" s="1" t="s">
+      <c r="V6" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="V6" s="1" t="s">
+      <c r="W6" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="W6" s="1" t="s">
+      <c r="X6" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="X6" s="1">
+      <c r="Y6" s="1">
         <v>123456</v>
       </c>
-      <c r="Y6" s="1" t="s">
+      <c r="Z6" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="Z6" s="1">
+      <c r="AA6" s="1">
         <v>450178</v>
       </c>
-      <c r="AA6" s="1" t="s">
+      <c r="AB6" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AB6" s="1" t="s">
+      <c r="AC6" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="AD6" s="1" t="s">
+      <c r="AE6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AE6" s="1" t="s">
+      <c r="AF6" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="AF6" s="1" t="s">
+      <c r="AG6" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="AG6" s="1" t="s">
+      <c r="AH6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AH6" s="1" t="s">
+      <c r="AI6" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AI6" s="1" t="s">
+      <c r="AJ6" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:35">
+    <row r="7" spans="1:36">
       <c r="A7" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="3"/>
+      <c r="C7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <v>15</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
         <v>5000000</v>
       </c>
-      <c r="F7" s="1">
+      <c r="G7" s="1">
         <v>15</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="1">
+      <c r="J7" s="1">
         <v>7854126980</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="M7" s="1">
+      <c r="N7" s="1">
         <v>1789654123012</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="O7" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="P7" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="P7" s="1">
+      <c r="Q7" s="1">
         <v>462015</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="R7" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="R7" s="1" t="s">
+      <c r="S7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="S7" s="1" t="s">
+      <c r="T7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="T7" s="1" t="s">
+      <c r="U7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="U7" s="1" t="s">
+      <c r="V7" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="V7" s="1" t="s">
+      <c r="W7" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="W7" s="1" t="s">
+      <c r="X7" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="X7" s="1">
+      <c r="Y7" s="1">
         <v>123456</v>
       </c>
-      <c r="Y7" s="1" t="s">
+      <c r="Z7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="Z7" s="1">
+      <c r="AA7" s="1">
         <v>450130</v>
       </c>
-      <c r="AA7" s="1" t="s">
+      <c r="AB7" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="AB7" s="1" t="s">
+      <c r="AC7" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="AD7" s="1" t="s">
+      <c r="AE7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AE7" s="1" t="s">
+      <c r="AF7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AF7" s="1" t="s">
+      <c r="AG7" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="AG7" s="1" t="s">
+      <c r="AH7" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AH7" s="1" t="s">
+      <c r="AI7" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AI7" s="1" t="s">
+      <c r="AJ7" s="1" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="G1:S2 A3:C4 A6:C6 G4:S7 A7:E7 A5:E5 A1:E2 H3:S3 T2:U3 Y1:AI1 W2:W7 T1:W1 Y2:AH7 U7 U4 U5 U6" numberStoredAsText="1"/>
+    <ignoredError sqref="H1:T2 C3:D4 C6:D6 H4:T7 C7:F7 C5:F5 C1:F2 I3:T3 U2:V3 Z1:AJ1 X2:X7 U1:X1 Z2:AI7 V4:V7 A1:A7" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>